<commit_message>
Fixes and price edit
</commit_message>
<xml_diff>
--- a/Relatorio-grp.xlsx
+++ b/Relatorio-grp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ru_da\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ru_da\GitHub\AINet_Project_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33DB6BC-12D2-4039-AF88-18BCBF4CF128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B98BCB-BC5F-4147-BA0F-C234F491D097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="d1dTnVKyZmOIMXAmVG8x5PmT/ohaZvLRwgKeLFIBaPCq2tDXm4mYgDGYIvygv/Rie4Lus3AATwu4xam55phyug==" workbookSaltValue="hRTEJqbbhrDw2liaZuJCSg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Nº Grupo</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Completo</t>
+  </si>
+  <si>
+    <t>Suporte para Laravel Localization</t>
   </si>
 </sst>
 </file>
@@ -452,14 +455,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
@@ -477,29 +489,20 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -818,7 +821,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26:I26"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14:I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -870,12 +873,12 @@
       <c r="E5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="38"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="29"/>
     </row>
     <row r="6" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
@@ -887,12 +890,12 @@
       <c r="E6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="36" t="s">
+      <c r="F6" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="38"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="29"/>
     </row>
     <row r="7" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
@@ -904,36 +907,36 @@
       <c r="E7" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="38"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="29"/>
     </row>
     <row r="8" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
     </row>
     <row r="10" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="6"/>
       <c r="C10" s="21"/>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="2:9" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
@@ -945,48 +948,48 @@
       <c r="I11" s="23"/>
     </row>
     <row r="12" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
     </row>
     <row r="13" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="34"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="34"/>
     </row>
     <row r="14" spans="2:9" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" spans="2:9" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
     </row>
     <row r="16" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
@@ -1001,14 +1004,16 @@
       <c r="C17" s="13"/>
     </row>
     <row r="18" spans="2:10" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
+      <c r="B18" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" spans="2:10" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
@@ -1027,42 +1032,42 @@
       <c r="C21" s="13"/>
     </row>
     <row r="22" spans="2:10" ht="129.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
-      <c r="I22" s="28"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="30"/>
+      <c r="I22" s="30"/>
     </row>
     <row r="24" spans="2:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
     </row>
     <row r="25" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="27" t="s">
+      <c r="D25" s="37"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
       <c r="J25" s="17" t="s">
         <v>27</v>
       </c>
@@ -1071,15 +1076,15 @@
       <c r="B26" s="4">
         <v>1</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
       <c r="J26" s="20" t="s">
         <v>17</v>
       </c>
@@ -1088,15 +1093,15 @@
       <c r="B27" s="4">
         <v>2</v>
       </c>
-      <c r="C27" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
+      <c r="C27" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
       <c r="J27" s="20" t="s">
         <v>18</v>
       </c>
@@ -1105,15 +1110,15 @@
       <c r="B28" s="4">
         <v>3</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="28"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
       <c r="J28" s="20" t="s">
         <v>19</v>
       </c>
@@ -1122,15 +1127,15 @@
       <c r="B29" s="4">
         <v>4</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
       <c r="J29" s="20" t="s">
         <v>20</v>
       </c>
@@ -1139,15 +1144,15 @@
       <c r="B30" s="4">
         <v>5</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="28"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="28"/>
-      <c r="I30" s="28"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="30"/>
+      <c r="I30" s="30"/>
       <c r="J30" s="20" t="s">
         <v>21</v>
       </c>
@@ -1156,15 +1161,15 @@
       <c r="B31" s="4">
         <v>6</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
       <c r="J31" s="20" t="s">
         <v>22</v>
       </c>
@@ -1173,15 +1178,15 @@
       <c r="B32" s="4">
         <v>7</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
-      <c r="I32" s="28"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="30"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
       <c r="J32" s="20" t="s">
         <v>23</v>
       </c>
@@ -1190,15 +1195,15 @@
       <c r="B33" s="4">
         <v>8</v>
       </c>
-      <c r="C33" s="29" t="s">
+      <c r="C33" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="28"/>
-      <c r="H33" s="28"/>
-      <c r="I33" s="28"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="30"/>
+      <c r="I33" s="30"/>
       <c r="J33" s="20" t="s">
         <v>24</v>
       </c>
@@ -1211,11 +1216,22 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="dFHhedqTgfvoMpuk4AU9VrMrwim7o71PPV4NSvy5W8VBc9L8onrWRxtOCmq5CfY4fQJThvLL9b5Fe9WH6rzUWg==" saltValue="gAxNU4QP/+ESVYRnPpuKiw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="30">
-    <mergeCell ref="B9:I9"/>
-    <mergeCell ref="E10:I10"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="C27:E27"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="C31:E31"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="C28:E28"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B14:I14"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="F28:I28"/>
@@ -1225,22 +1241,11 @@
     <mergeCell ref="F30:I30"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="F32:I32"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="C27:E27"/>
-    <mergeCell ref="F27:I27"/>
-    <mergeCell ref="C31:E31"/>
-    <mergeCell ref="F31:I31"/>
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="B24:I24"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="E10:I10"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="F7:I7"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="C26:E33">

</xml_diff>